<commit_message>
change dropdown into input tag
</commit_message>
<xml_diff>
--- a/backend/students.xlsx
+++ b/backend/students.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Batch</t>
   </si>
@@ -28,46 +28,19 @@
     <t>Institute</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>xyz</t>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>btcs</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>1245679935</t>
-  </si>
-  <si>
-    <t>Institute 3</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>123456789</t>
+    <t>1234567890</t>
   </si>
   <si>
     <t>Institute 1</t>
-  </si>
-  <si>
-    <t>b.tech</t>
-  </si>
-  <si>
-    <t>cse</t>
-  </si>
-  <si>
-    <t>1236547890</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>Institute 2</t>
-  </si>
-  <si>
-    <t>123466</t>
   </si>
 </sst>
 </file>
@@ -444,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="20" customWidth="1"/>
@@ -484,74 +457,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>